<commit_message>
Refactor student DTOs and schemas, and add excel options
</commit_message>
<xml_diff>
--- a/server/students-all.xlsx
+++ b/server/students-all.xlsx
@@ -4,10 +4,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="CA" sheetId="1" r:id="rId1"/>
-    <sheet name="SJ" sheetId="2" r:id="rId2"/>
-    <sheet name="SC" sheetId="3" r:id="rId3"/>
-    <sheet name="AL" sheetId="4" r:id="rId4"/>
-    <sheet name="LI" sheetId="5" r:id="rId5"/>
+    <sheet name="AL" sheetId="2" r:id="rId2"/>
+    <sheet name="SJ" sheetId="3" r:id="rId3"/>
+    <sheet name="LI" sheetId="4" r:id="rId4"/>
+    <sheet name="SC" sheetId="5" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
@@ -401,39 +401,586 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>carnet</v>
+      </c>
+      <c r="B1" t="str">
+        <v>name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>email</v>
+      </c>
+      <c r="D1" t="str">
+        <v>personalPNumber</v>
+      </c>
+      <c r="E1" t="str">
+        <v>campus</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>346370</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Student1</v>
+      </c>
+      <c r="C2" t="str">
+        <v>email1</v>
+      </c>
+      <c r="D2" t="str">
+        <v>1000000</v>
+      </c>
+      <c r="E2" t="str">
+        <v>CA</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>558960</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Student2</v>
+      </c>
+      <c r="C3" t="str">
+        <v>email2</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2000000</v>
+      </c>
+      <c r="E3" t="str">
+        <v>CA</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>8707</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Student3</v>
+      </c>
+      <c r="C4" t="str">
+        <v>email3</v>
+      </c>
+      <c r="D4" t="str">
+        <v>3000000</v>
+      </c>
+      <c r="E4" t="str">
+        <v>CA</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>896451</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Student4</v>
+      </c>
+      <c r="C5" t="str">
+        <v>email4</v>
+      </c>
+      <c r="D5" t="str">
+        <v>4000000</v>
+      </c>
+      <c r="E5" t="str">
+        <v>CA</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>153491</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Student5</v>
+      </c>
+      <c r="C6" t="str">
+        <v>email5</v>
+      </c>
+      <c r="D6" t="str">
+        <v>5000000</v>
+      </c>
+      <c r="E6" t="str">
+        <v>CA</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>29284</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Student6</v>
+      </c>
+      <c r="C7" t="str">
+        <v>email6</v>
+      </c>
+      <c r="D7" t="str">
+        <v>6000000</v>
+      </c>
+      <c r="E7" t="str">
+        <v>CA</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>436733</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Student7</v>
+      </c>
+      <c r="C8" t="str">
+        <v>email7</v>
+      </c>
+      <c r="D8" t="str">
+        <v>7000000</v>
+      </c>
+      <c r="E8" t="str">
+        <v>CA</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>314231</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Student8</v>
+      </c>
+      <c r="C9" t="str">
+        <v>email8</v>
+      </c>
+      <c r="D9" t="str">
+        <v>8000000</v>
+      </c>
+      <c r="E9" t="str">
+        <v>CA</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>945068</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Student9</v>
+      </c>
+      <c r="C10" t="str">
+        <v>email9</v>
+      </c>
+      <c r="D10" t="str">
+        <v>9000000</v>
+      </c>
+      <c r="E10" t="str">
+        <v>CA</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E10"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>carnet</v>
+      </c>
+      <c r="B1" t="str">
+        <v>name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>email</v>
+      </c>
+      <c r="D1" t="str">
+        <v>personalPNumber</v>
+      </c>
+      <c r="E1" t="str">
+        <v>campus</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>531259</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Student0</v>
+      </c>
+      <c r="C2" t="str">
+        <v>email0</v>
+      </c>
+      <c r="D2" t="str">
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <v>AL</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>346370</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Student1</v>
+      </c>
+      <c r="C3" t="str">
+        <v>email1</v>
+      </c>
+      <c r="D3" t="str">
+        <v>1000000</v>
+      </c>
+      <c r="E3" t="str">
+        <v>AL</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>558960</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Student2</v>
+      </c>
+      <c r="C4" t="str">
+        <v>email2</v>
+      </c>
+      <c r="D4" t="str">
+        <v>2000000</v>
+      </c>
+      <c r="E4" t="str">
+        <v>AL</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>8707</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Student3</v>
+      </c>
+      <c r="C5" t="str">
+        <v>email3</v>
+      </c>
+      <c r="D5" t="str">
+        <v>3000000</v>
+      </c>
+      <c r="E5" t="str">
+        <v>AL</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>896451</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Student4</v>
+      </c>
+      <c r="C6" t="str">
+        <v>email4</v>
+      </c>
+      <c r="D6" t="str">
+        <v>4000000</v>
+      </c>
+      <c r="E6" t="str">
+        <v>AL</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>153491</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Student5</v>
+      </c>
+      <c r="C7" t="str">
+        <v>email5</v>
+      </c>
+      <c r="D7" t="str">
+        <v>5000000</v>
+      </c>
+      <c r="E7" t="str">
+        <v>AL</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>29284</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Student6</v>
+      </c>
+      <c r="C8" t="str">
+        <v>email6</v>
+      </c>
+      <c r="D8" t="str">
+        <v>6000000</v>
+      </c>
+      <c r="E8" t="str">
+        <v>AL</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>436733</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Student7</v>
+      </c>
+      <c r="C9" t="str">
+        <v>email7</v>
+      </c>
+      <c r="D9" t="str">
+        <v>7000000</v>
+      </c>
+      <c r="E9" t="str">
+        <v>AL</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>314231</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Student8</v>
+      </c>
+      <c r="C10" t="str">
+        <v>email8</v>
+      </c>
+      <c r="D10" t="str">
+        <v>8000000</v>
+      </c>
+      <c r="E10" t="str">
+        <v>AL</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>945068</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Student9</v>
+      </c>
+      <c r="C11" t="str">
+        <v>email9</v>
+      </c>
+      <c r="D11" t="str">
+        <v>9000000</v>
+      </c>
+      <c r="E11" t="str">
+        <v>AL</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E11"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>carnet</v>
+      </c>
+      <c r="B1" t="str">
+        <v>name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>email</v>
+      </c>
+      <c r="D1" t="str">
+        <v>personalPNumber</v>
+      </c>
+      <c r="E1" t="str">
+        <v>campus</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>531259</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Student0</v>
+      </c>
+      <c r="C2" t="str">
+        <v>email0</v>
+      </c>
+      <c r="D2" t="str">
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <v>SJ</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>346370</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Student1</v>
+      </c>
+      <c r="C3" t="str">
+        <v>email1</v>
+      </c>
+      <c r="D3" t="str">
+        <v>1000000</v>
+      </c>
+      <c r="E3" t="str">
+        <v>SJ</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>558960</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Student2</v>
+      </c>
+      <c r="C4" t="str">
+        <v>email2</v>
+      </c>
+      <c r="D4" t="str">
+        <v>2000000</v>
+      </c>
+      <c r="E4" t="str">
+        <v>SJ</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>8707</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Student3</v>
+      </c>
+      <c r="C5" t="str">
+        <v>email3</v>
+      </c>
+      <c r="D5" t="str">
+        <v>3000000</v>
+      </c>
+      <c r="E5" t="str">
+        <v>SJ</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>896451</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Student4</v>
+      </c>
+      <c r="C6" t="str">
+        <v>email4</v>
+      </c>
+      <c r="D6" t="str">
+        <v>4000000</v>
+      </c>
+      <c r="E6" t="str">
+        <v>SJ</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>153491</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Student5</v>
+      </c>
+      <c r="C7" t="str">
+        <v>email5</v>
+      </c>
+      <c r="D7" t="str">
+        <v>5000000</v>
+      </c>
+      <c r="E7" t="str">
+        <v>SJ</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>29284</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Student6</v>
+      </c>
+      <c r="C8" t="str">
+        <v>email6</v>
+      </c>
+      <c r="D8" t="str">
+        <v>6000000</v>
+      </c>
+      <c r="E8" t="str">
+        <v>SJ</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>436733</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Student7</v>
+      </c>
+      <c r="C9" t="str">
+        <v>email7</v>
+      </c>
+      <c r="D9" t="str">
+        <v>7000000</v>
+      </c>
+      <c r="E9" t="str">
+        <v>SJ</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>314231</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Student8</v>
+      </c>
+      <c r="C10" t="str">
+        <v>email8</v>
+      </c>
+      <c r="D10" t="str">
+        <v>8000000</v>
+      </c>
+      <c r="E10" t="str">
+        <v>SJ</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>945068</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Student9</v>
+      </c>
+      <c r="C11" t="str">
+        <v>email9</v>
+      </c>
+      <c r="D11" t="str">
+        <v>9000000</v>
+      </c>
+      <c r="E11" t="str">
+        <v>SJ</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E11"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>